<commit_message>
minor change to deleting and displaying
</commit_message>
<xml_diff>
--- a/data/breaks.xlsx
+++ b/data/breaks.xlsx
@@ -7,30 +7,10 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>cd</t>
-  </si>
-  <si>
-    <t>2025-01-19T03:41</t>
-  </si>
-  <si>
-    <t>2025-01-13T03:41</t>
-  </si>
-  <si>
-    <t>2025-01-13T02:41</t>
-  </si>
-  <si>
-    <t>ed</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,7 +352,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -383,36 +363,7 @@
     <col min="3" max="3" width="6.719285714285714" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.719285714285713" style="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
timline displaying breaks in 1 row
</commit_message>
<xml_diff>
--- a/data/breaks.xlsx
+++ b/data/breaks.xlsx
@@ -14,18 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>AS</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>2025-01-14T04:22</t>
-  </si>
-  <si>
-    <t>2025-01-14T03:22</t>
+    <t>2025-01-14T12:00</t>
+  </si>
+  <si>
+    <t>2025-01-14T11:00</t>
+  </si>
+  <si>
+    <t>2025-01-14T13:00</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>2025-01-14T15:20</t>
+  </si>
+  <si>
+    <t>2025-01-14T17:30</t>
+  </si>
+  <si>
+    <t>2025-01-14T19:20</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>2025-01-14T11:50</t>
+  </si>
+  <si>
+    <t>2025-01-14T14:30</t>
   </si>
 </sst>
 </file>
@@ -369,7 +390,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D5" sqref="D5"/>
@@ -387,28 +408,42 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
-        <v>2</v>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colour scheme changed. Breaks displaying on individual rows per CX rep
</commit_message>
<xml_diff>
--- a/data/breaks.xlsx
+++ b/data/breaks.xlsx
@@ -14,39 +14,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+  <si>
+    <t>BSP</t>
+  </si>
+  <si>
+    <t>2025-01-19T11:25</t>
+  </si>
+  <si>
+    <t>2025-01-19T12:30</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>2025-01-19T11:50</t>
+  </si>
+  <si>
+    <t>2025-01-19T13:00</t>
+  </si>
+  <si>
+    <t>2025-01-19T15:30</t>
+  </si>
   <si>
     <t>AS</t>
   </si>
   <si>
-    <t>2025-01-14T12:00</t>
-  </si>
-  <si>
-    <t>2025-01-14T11:00</t>
-  </si>
-  <si>
-    <t>2025-01-14T13:00</t>
-  </si>
-  <si>
-    <t>EM</t>
-  </si>
-  <si>
-    <t>2025-01-14T15:20</t>
-  </si>
-  <si>
-    <t>2025-01-14T17:30</t>
-  </si>
-  <si>
-    <t>2025-01-14T19:20</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>2025-01-14T11:50</t>
-  </si>
-  <si>
-    <t>2025-01-14T14:30</t>
+    <t>2025-01-19T12:20</t>
+  </si>
+  <si>
+    <t>2025-01-19T14:30</t>
+  </si>
+  <si>
+    <t>2025-01-19T15:20</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>2025-01-19T17:00</t>
+  </si>
+  <si>
+    <t>2025-01-19T20:00</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>2025-01-19T21:30</t>
+  </si>
+  <si>
+    <t>2025-01-19T23:00</t>
+  </si>
+  <si>
+    <t>2025-01-19T00:00</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>2025-01-19T18:30</t>
+  </si>
+  <si>
+    <t>2025-01-19T21:00</t>
+  </si>
+  <si>
+    <t>2025-01-19T23:30</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>2025-01-19T19:30</t>
+  </si>
+  <si>
+    <t>2025-01-19T21:40</t>
+  </si>
+  <si>
+    <t>2025-01-19T23:50</t>
   </si>
 </sst>
 </file>
@@ -390,7 +438,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D5" sqref="D5"/>
@@ -443,7 +491,63 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
breaks now in single line and overlapping breaks move to 1 extra layer
</commit_message>
<xml_diff>
--- a/data/breaks.xlsx
+++ b/data/breaks.xlsx
@@ -14,87 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
-  <si>
-    <t>BSP</t>
-  </si>
-  <si>
-    <t>2025-01-19T11:25</t>
-  </si>
-  <si>
-    <t>2025-01-19T12:30</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>2025-01-21T11:50</t>
+  </si>
+  <si>
+    <t>2025-01-21T12:30</t>
+  </si>
+  <si>
+    <t>2025-01-21T14:50</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>2025-01-21T12:10</t>
+  </si>
+  <si>
+    <t>2025-01-21T14:30</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>2025-01-19T11:50</t>
-  </si>
-  <si>
-    <t>2025-01-19T13:00</t>
-  </si>
-  <si>
-    <t>2025-01-19T15:30</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>2025-01-19T12:20</t>
-  </si>
-  <si>
-    <t>2025-01-19T14:30</t>
-  </si>
-  <si>
-    <t>2025-01-19T15:20</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>2025-01-19T17:00</t>
-  </si>
-  <si>
-    <t>2025-01-19T20:00</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>2025-01-19T21:30</t>
-  </si>
-  <si>
-    <t>2025-01-19T23:00</t>
-  </si>
-  <si>
-    <t>2025-01-19T00:00</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>2025-01-19T18:30</t>
-  </si>
-  <si>
-    <t>2025-01-19T21:00</t>
-  </si>
-  <si>
-    <t>2025-01-19T23:30</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>2025-01-19T19:30</t>
-  </si>
-  <si>
-    <t>2025-01-19T21:40</t>
-  </si>
-  <si>
-    <t>2025-01-19T23:50</t>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>2025-01-21T12:20</t>
   </si>
 </sst>
 </file>
@@ -438,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D5" sqref="D5"/>
@@ -485,69 +434,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added colour picker with some colour options. Excel spreadsheet now stores colour value also.
</commit_message>
<xml_diff>
--- a/data/breaks.xlsx
+++ b/data/breaks.xlsx
@@ -14,36 +14,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>AS</t>
   </si>
   <si>
-    <t>2025-01-21T11:50</t>
-  </si>
-  <si>
-    <t>2025-01-21T12:30</t>
-  </si>
-  <si>
-    <t>2025-01-21T14:50</t>
-  </si>
-  <si>
-    <t>EM</t>
-  </si>
-  <si>
-    <t>2025-01-21T12:10</t>
-  </si>
-  <si>
-    <t>2025-01-21T14:30</t>
+    <t>2025-02-03T11:30</t>
+  </si>
+  <si>
+    <t>2025-02-03T13:00</t>
+  </si>
+  <si>
+    <t>2025-02-03T14:50</t>
+  </si>
+  <si>
+    <t>2025-02-04T14:24</t>
+  </si>
+  <si>
+    <t>2025-02-04T16:25</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:25</t>
+  </si>
+  <si>
+    <t>rgb(30, 144, 255)</t>
+  </si>
+  <si>
+    <t>2025-02-04T15:24</t>
+  </si>
+  <si>
+    <t>2025-02-04T18:25</t>
+  </si>
+  <si>
+    <t>rgb(46, 139, 87)</t>
+  </si>
+  <si>
+    <t>2025-02-06T12:28</t>
+  </si>
+  <si>
+    <t>2025-02-04T14:28</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>2025-01-21T12:20</t>
+    <t>rgb(194, 24, 7)</t>
+  </si>
+  <si>
+    <t>2025-02-06T11:28</t>
+  </si>
+  <si>
+    <t>2025-02-04T15:28</t>
+  </si>
+  <si>
+    <t>rgb(241, 156, 187)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +411,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="D5" sqref="D5"/>
@@ -415,32 +439,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>